<commit_message>
feat: Add initial implementation of 2D plot for EPS
</commit_message>
<xml_diff>
--- a/n-k.xlsx
+++ b/n-k.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugm365-my.sharepoint.com/personal/muhammadfaliqadlan_365_ugm_ac_id/Documents/fdtd-python/code-fdtd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{C964F8B6-469F-45FD-9EF4-8C5F19903317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44A0B6DD-3344-44B4-B512-F69F2B7EAD01}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{C964F8B6-469F-45FD-9EF4-8C5F19903317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2067137B-62FA-4CFA-B1D3-AEA9A6D362F4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10D65F64-FF1D-4BD0-97B5-63B011C857F4}"/>
   </bookViews>
@@ -4642,16 +4642,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>154457</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>156816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>459257</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>156816</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4998,8 +4998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A85291C-36BE-4A60-95C5-D81510C653AC}">
   <dimension ref="A1:AG600"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>